<commit_message>
addNew, Update, delete, import new table
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.Catalogue/eFMS.API.Catalogue/Resources/Files/DistrictImportTemplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.Catalogue/eFMS.API.Catalogue/Resources/Files/DistrictImportTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\efms\src\WebAPI\eFMS.API.SystemWeb\CatalogueManagement\eFMS.API.Catalogue\Resources\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intern.lth009\Documents\eFMS-WebApp\WebAPI\eFMS.API.SystemWeb\eFMS.API.Catalogue\eFMS.API.Catalogue\Resources\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>English Name</t>
   </si>
@@ -32,29 +32,41 @@
     <t>Local Name</t>
   </si>
   <si>
-    <t>Country</t>
-  </si>
-  <si>
     <t>Inactive</t>
   </si>
   <si>
     <t>District Code</t>
   </si>
   <si>
-    <t>Province</t>
-  </si>
-  <si>
-    <t>Quận Ba Đình</t>
-  </si>
-  <si>
-    <t>Thành phố Hà Nội</t>
+    <t>Country Code</t>
+  </si>
+  <si>
+    <t>Province Code</t>
+  </si>
+  <si>
+    <t>VN039020001</t>
+  </si>
+  <si>
+    <t>Gò Vấp</t>
+  </si>
+  <si>
+    <t>Quận Gò Vấp</t>
+  </si>
+  <si>
+    <t>VN</t>
+  </si>
+  <si>
+    <t>HCM</t>
+  </si>
+  <si>
+    <t>Active</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +79,11 @@
       <sz val="11"/>
       <name val="Century Gothic"/>
       <family val="4"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF212529"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,12 +121,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,22 +408,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="B2:D2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.7265625" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="42.54296875" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -414,49 +434,42 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6">
       <c r="C4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6">
       <c r="C5" s="2"/>
       <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C8" s="2"/>
-      <c r="E8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>